<commit_message>
Actualizacion del Indice con tonalidad, ritmo, y numero de estrofas.
</commit_message>
<xml_diff>
--- a/Indice.xlsx
+++ b/Indice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EPV\Desktop\D'Aaron\Curso de Python\Hymn_List_Manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D'Aaron\Curso de Python\Hymn_List_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$P$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$O$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="203">
   <si>
     <t>Oh Santisimo Oh Felicísimo</t>
   </si>
@@ -565,13 +565,166 @@
   </si>
   <si>
     <t>Oh Ven Emanuel</t>
+  </si>
+  <si>
+    <t>Ritmo</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>2/2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>4/4</t>
+  </si>
+  <si>
+    <t>Ab</t>
+  </si>
+  <si>
+    <t>2/4</t>
+  </si>
+  <si>
+    <t>Bb</t>
+  </si>
+  <si>
+    <t>6/8</t>
+  </si>
+  <si>
+    <t>9/8</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Eb</t>
+  </si>
+  <si>
+    <t>3/4</t>
+  </si>
+  <si>
+    <t>Tn.</t>
+  </si>
+  <si>
+    <t>9/4</t>
+  </si>
+  <si>
+    <t>N°E.</t>
+  </si>
+  <si>
+    <t>Fm</t>
+  </si>
+  <si>
+    <t>6/4</t>
+  </si>
+  <si>
+    <t>3/2</t>
+  </si>
+  <si>
+    <t>Db</t>
+  </si>
+  <si>
+    <t>Ab/Bb/C</t>
+  </si>
+  <si>
+    <t>4/8</t>
+  </si>
+  <si>
+    <t>12/8 - 9/8</t>
+  </si>
+  <si>
+    <t>Gb/Ab</t>
+  </si>
+  <si>
+    <t>4(5)</t>
+  </si>
+  <si>
+    <t>G/A</t>
+  </si>
+  <si>
+    <t>Eb/F</t>
+  </si>
+  <si>
+    <t>C/D</t>
+  </si>
+  <si>
+    <t>3/2+2/2</t>
+  </si>
+  <si>
+    <t>Em</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Escritor</t>
+  </si>
+  <si>
+    <t>William J. Gaither</t>
+  </si>
+  <si>
+    <t>Gloria y William J. Gaither</t>
+  </si>
+  <si>
+    <t>Rowland F. Prichard</t>
+  </si>
+  <si>
+    <t>William C. Dix</t>
+  </si>
+  <si>
+    <t>Tomas. J. Williams</t>
+  </si>
+  <si>
+    <t>S. Trevor Francis</t>
+  </si>
+  <si>
+    <t>Ron Hamilton</t>
+  </si>
+  <si>
+    <t>Matt Merker</t>
+  </si>
+  <si>
+    <t>Ada Habershon</t>
+  </si>
+  <si>
+    <t>William H. Monk</t>
+  </si>
+  <si>
+    <t>Henry F. Lyte</t>
+  </si>
+  <si>
+    <t>Charles F. Weigle</t>
+  </si>
+  <si>
+    <t>Ruth Caye Jones</t>
+  </si>
+  <si>
+    <t>Tomas Campbell</t>
+  </si>
+  <si>
+    <t>Charles Wesley</t>
+  </si>
+  <si>
+    <t>George Beverly Shea</t>
+  </si>
+  <si>
+    <t>Rhea F. Miller</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,6 +812,13 @@
       <b/>
       <sz val="11"/>
       <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -776,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,11 +1048,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,10 +1356,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q148"/>
+  <dimension ref="A1:P148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="J137" sqref="J137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,17 +1369,16 @@
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="5" width="6.7109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" style="50" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" style="50" customWidth="1"/>
-    <col min="9" max="10" width="6.7109375" style="50" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="50" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" style="50" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" style="50" customWidth="1"/>
-    <col min="14" max="15" width="6.7109375" style="50" customWidth="1"/>
-    <col min="16" max="16" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="54" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="55" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="54" customWidth="1"/>
+    <col min="10" max="11" width="17" style="50" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" style="50" customWidth="1"/>
+    <col min="13" max="14" width="6.7109375" style="50" customWidth="1"/>
+    <col min="15" max="15" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="45"/>
       <c r="C1" s="35" t="s">
@@ -1214,19 +1393,28 @@
       <c r="F1" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="48"/>
+      <c r="G1" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="48"/>
+      <c r="M1" s="49"/>
       <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
+      <c r="O1" s="18"/>
       <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="20"/>
       <c r="C2" s="25" t="s">
@@ -1239,19 +1427,24 @@
       <c r="F2" s="20">
         <v>112</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="G2" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="15">
+        <v>4</v>
+      </c>
       <c r="J2" s="46"/>
       <c r="K2" s="46"/>
       <c r="L2" s="46"/>
       <c r="M2" s="46"/>
       <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="O2" s="18"/>
       <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="52"/>
       <c r="C3" s="25" t="s">
@@ -1264,19 +1457,24 @@
       <c r="F3" s="20">
         <v>2</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="G3" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="52">
+        <v>3</v>
+      </c>
       <c r="J3" s="46"/>
       <c r="K3" s="46"/>
       <c r="L3" s="46"/>
       <c r="M3" s="46"/>
       <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
+      <c r="O3" s="18"/>
       <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="20"/>
       <c r="C4" s="24" t="s">
@@ -1291,19 +1489,24 @@
       <c r="F4" s="20">
         <v>3</v>
       </c>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
+      <c r="G4" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" s="52">
+        <v>4</v>
+      </c>
       <c r="J4" s="46"/>
       <c r="K4" s="46"/>
       <c r="L4" s="46"/>
       <c r="M4" s="46"/>
       <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
+      <c r="O4" s="18"/>
       <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="20"/>
       <c r="C5" s="24" t="s">
@@ -1316,19 +1519,24 @@
       <c r="F5" s="20">
         <v>4</v>
       </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="G5" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="60" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="52">
+        <v>3</v>
+      </c>
       <c r="J5" s="46"/>
       <c r="K5" s="46"/>
       <c r="L5" s="46"/>
       <c r="M5" s="46"/>
       <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
+      <c r="O5" s="18"/>
       <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="20"/>
       <c r="C6" s="27" t="s">
@@ -1343,19 +1551,24 @@
       <c r="F6" s="21">
         <v>5</v>
       </c>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
+      <c r="G6" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I6" s="52">
+        <v>4</v>
+      </c>
       <c r="J6" s="46"/>
       <c r="K6" s="46"/>
       <c r="L6" s="46"/>
       <c r="M6" s="46"/>
       <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
+      <c r="O6" s="18"/>
       <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="52"/>
       <c r="C7" s="27" t="s">
@@ -1370,19 +1583,24 @@
       <c r="F7" s="20">
         <v>6</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="G7" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="52">
+        <v>3</v>
+      </c>
       <c r="J7" s="46"/>
       <c r="K7" s="46"/>
       <c r="L7" s="46"/>
       <c r="M7" s="46"/>
       <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
+      <c r="O7" s="18"/>
       <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="20"/>
       <c r="C8" s="23" t="s">
@@ -1395,19 +1613,24 @@
       <c r="F8" s="20">
         <v>7</v>
       </c>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="G8" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" s="52">
+        <v>3</v>
+      </c>
       <c r="J8" s="46"/>
       <c r="K8" s="46"/>
       <c r="L8" s="46"/>
       <c r="M8" s="46"/>
       <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
+      <c r="O8" s="18"/>
       <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="20"/>
       <c r="C9" s="24" t="s">
@@ -1420,19 +1643,24 @@
       <c r="F9" s="20">
         <v>8</v>
       </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="G9" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" s="52">
+        <v>3</v>
+      </c>
       <c r="J9" s="46"/>
       <c r="K9" s="46"/>
       <c r="L9" s="46"/>
       <c r="M9" s="46"/>
       <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
+      <c r="O9" s="18"/>
       <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="20"/>
       <c r="C10" s="24" t="s">
@@ -1445,19 +1673,24 @@
       <c r="F10" s="21">
         <v>9</v>
       </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="G10" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H10" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" s="52">
+        <v>3</v>
+      </c>
       <c r="J10" s="46"/>
       <c r="K10" s="46"/>
       <c r="L10" s="46"/>
       <c r="M10" s="46"/>
       <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
+      <c r="O10" s="18"/>
       <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="20"/>
       <c r="C11" s="25" t="s">
@@ -1470,19 +1703,24 @@
       <c r="F11" s="20">
         <v>10</v>
       </c>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
+      <c r="G11" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I11" s="52">
+        <v>3</v>
+      </c>
       <c r="J11" s="46"/>
       <c r="K11" s="46"/>
       <c r="L11" s="46"/>
       <c r="M11" s="46"/>
       <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
+      <c r="O11" s="18"/>
       <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="52"/>
       <c r="C12" s="30" t="s">
@@ -1497,19 +1735,24 @@
       <c r="F12" s="20">
         <v>11</v>
       </c>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
+      <c r="G12" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" s="52">
+        <v>4</v>
+      </c>
       <c r="J12" s="46"/>
       <c r="K12" s="46"/>
       <c r="L12" s="46"/>
       <c r="M12" s="46"/>
       <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
+      <c r="O12" s="18"/>
       <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="52"/>
       <c r="C13" s="27" t="s">
@@ -1524,19 +1767,24 @@
       <c r="F13" s="20">
         <v>12</v>
       </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
+      <c r="G13" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="52">
+        <v>3</v>
+      </c>
       <c r="J13" s="46"/>
       <c r="K13" s="46"/>
       <c r="L13" s="46"/>
       <c r="M13" s="46"/>
       <c r="N13" s="46"/>
-      <c r="O13" s="46"/>
+      <c r="O13" s="18"/>
       <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="52"/>
       <c r="C14" s="25" t="s">
@@ -1551,19 +1799,24 @@
       <c r="F14" s="20">
         <v>13</v>
       </c>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
+      <c r="G14" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" s="52">
+        <v>3</v>
+      </c>
       <c r="J14" s="46"/>
       <c r="K14" s="46"/>
       <c r="L14" s="46"/>
       <c r="M14" s="46"/>
       <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
+      <c r="O14" s="18"/>
       <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
       <c r="B15" s="52"/>
       <c r="C15" s="23" t="s">
@@ -1578,19 +1831,24 @@
       <c r="F15" s="20">
         <v>14</v>
       </c>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
+      <c r="G15" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15" s="52">
+        <v>4</v>
+      </c>
       <c r="J15" s="46"/>
       <c r="K15" s="46"/>
       <c r="L15" s="46"/>
       <c r="M15" s="46"/>
       <c r="N15" s="46"/>
-      <c r="O15" s="46"/>
+      <c r="O15" s="18"/>
       <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="52"/>
       <c r="C16" s="25" t="s">
@@ -1603,19 +1861,24 @@
       <c r="F16" s="20">
         <v>15</v>
       </c>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
+      <c r="G16" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" s="52">
+        <v>4</v>
+      </c>
       <c r="J16" s="46"/>
       <c r="K16" s="46"/>
       <c r="L16" s="46"/>
       <c r="M16" s="46"/>
       <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
+      <c r="O16" s="18"/>
       <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="52"/>
       <c r="C17" s="25" t="s">
@@ -1628,19 +1891,24 @@
       <c r="F17" s="20">
         <v>16</v>
       </c>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="G17" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I17" s="52">
+        <v>4</v>
+      </c>
       <c r="J17" s="46"/>
       <c r="K17" s="46"/>
       <c r="L17" s="46"/>
       <c r="M17" s="46"/>
       <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
+      <c r="O17" s="18"/>
       <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="17"/>
       <c r="B18" s="20"/>
       <c r="C18" s="27" t="s">
@@ -1655,19 +1923,24 @@
       <c r="F18" s="20">
         <v>17</v>
       </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
+      <c r="G18" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="H18" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I18" s="52">
+        <v>4</v>
+      </c>
       <c r="J18" s="46"/>
       <c r="K18" s="46"/>
       <c r="L18" s="46"/>
       <c r="M18" s="46"/>
       <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
+      <c r="O18" s="18"/>
       <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
       <c r="B19" s="20"/>
       <c r="C19" s="24" t="s">
@@ -1682,19 +1955,24 @@
       <c r="F19" s="20">
         <v>18</v>
       </c>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
+      <c r="G19" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I19" s="52">
+        <v>3</v>
+      </c>
       <c r="J19" s="46"/>
       <c r="K19" s="46"/>
       <c r="L19" s="46"/>
       <c r="M19" s="46"/>
       <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
+      <c r="O19" s="18"/>
       <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="B20" s="20"/>
       <c r="C20" s="27" t="s">
@@ -1709,19 +1987,24 @@
       <c r="F20" s="20">
         <v>19</v>
       </c>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
+      <c r="G20" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" s="52">
+        <v>3</v>
+      </c>
       <c r="J20" s="46"/>
       <c r="K20" s="46"/>
       <c r="L20" s="46"/>
       <c r="M20" s="46"/>
       <c r="N20" s="46"/>
-      <c r="O20" s="46"/>
+      <c r="O20" s="18"/>
       <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
       <c r="B21" s="52"/>
       <c r="C21" s="27" t="s">
@@ -1736,19 +2019,24 @@
       <c r="F21" s="20">
         <v>20</v>
       </c>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
+      <c r="G21" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="H21" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I21" s="52">
+        <v>4</v>
+      </c>
       <c r="J21" s="46"/>
       <c r="K21" s="46"/>
       <c r="L21" s="46"/>
       <c r="M21" s="46"/>
       <c r="N21" s="46"/>
-      <c r="O21" s="46"/>
+      <c r="O21" s="18"/>
       <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
       <c r="B22" s="20"/>
       <c r="C22" s="24" t="s">
@@ -1761,19 +2049,24 @@
       <c r="F22" s="20">
         <v>21</v>
       </c>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="G22" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H22" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I22" s="52">
+        <v>4</v>
+      </c>
       <c r="J22" s="46"/>
       <c r="K22" s="46"/>
       <c r="L22" s="46"/>
       <c r="M22" s="46"/>
       <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
+      <c r="O22" s="18"/>
       <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="17"/>
       <c r="B23" s="20"/>
       <c r="C23" s="27" t="s">
@@ -1788,19 +2081,24 @@
       <c r="F23" s="20">
         <v>22</v>
       </c>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
+      <c r="G23" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="52">
+        <v>3</v>
+      </c>
       <c r="J23" s="46"/>
       <c r="K23" s="46"/>
       <c r="L23" s="46"/>
       <c r="M23" s="46"/>
       <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
+      <c r="O23" s="18"/>
       <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="17"/>
       <c r="B24" s="20"/>
       <c r="C24" s="23" t="s">
@@ -1815,19 +2113,24 @@
       <c r="F24" s="20">
         <v>23</v>
       </c>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="G24" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H24" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" s="52">
+        <v>4</v>
+      </c>
       <c r="J24" s="46"/>
       <c r="K24" s="46"/>
       <c r="L24" s="46"/>
       <c r="M24" s="46"/>
       <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
+      <c r="O24" s="18"/>
       <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="52"/>
       <c r="C25" s="30" t="s">
@@ -1840,19 +2143,24 @@
       <c r="F25" s="20">
         <v>24</v>
       </c>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
+      <c r="G25" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" s="52">
+        <v>3</v>
+      </c>
       <c r="J25" s="46"/>
       <c r="K25" s="46"/>
       <c r="L25" s="46"/>
       <c r="M25" s="46"/>
       <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
+      <c r="O25" s="18"/>
       <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
       <c r="B26" s="52"/>
       <c r="C26" s="24" t="s">
@@ -1865,19 +2173,24 @@
       <c r="F26" s="20">
         <v>25</v>
       </c>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
+      <c r="G26" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="H26" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I26" s="52">
+        <v>3</v>
+      </c>
       <c r="J26" s="46"/>
       <c r="K26" s="46"/>
       <c r="L26" s="46"/>
       <c r="M26" s="46"/>
       <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
+      <c r="O26" s="18"/>
       <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="20"/>
       <c r="C27" s="24" t="s">
@@ -1890,19 +2203,24 @@
       <c r="F27" s="20">
         <v>26</v>
       </c>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
+      <c r="G27" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I27" s="52">
+        <v>3</v>
+      </c>
       <c r="J27" s="46"/>
       <c r="K27" s="46"/>
       <c r="L27" s="46"/>
       <c r="M27" s="46"/>
       <c r="N27" s="46"/>
-      <c r="O27" s="46"/>
+      <c r="O27" s="18"/>
       <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="17"/>
       <c r="B28" s="52"/>
       <c r="C28" s="25" t="s">
@@ -1917,19 +2235,24 @@
       <c r="F28" s="20">
         <v>27</v>
       </c>
-      <c r="G28" s="46"/>
-      <c r="H28" s="46"/>
-      <c r="I28" s="46"/>
+      <c r="G28" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H28" s="60" t="s">
+        <v>171</v>
+      </c>
+      <c r="I28" s="52">
+        <v>3</v>
+      </c>
       <c r="J28" s="46"/>
       <c r="K28" s="46"/>
       <c r="L28" s="46"/>
       <c r="M28" s="46"/>
       <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
+      <c r="O28" s="18"/>
       <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
       <c r="B29" s="52"/>
       <c r="C29" s="30" t="s">
@@ -1942,19 +2265,24 @@
       <c r="F29" s="20">
         <v>28</v>
       </c>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
+      <c r="G29" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I29" s="52">
+        <v>3</v>
+      </c>
       <c r="J29" s="46"/>
       <c r="K29" s="46"/>
       <c r="L29" s="46"/>
       <c r="M29" s="46"/>
       <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
+      <c r="O29" s="18"/>
       <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="20"/>
       <c r="C30" s="24" t="s">
@@ -1969,19 +2297,24 @@
       <c r="F30" s="20">
         <v>29</v>
       </c>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
+      <c r="G30" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I30" s="52">
+        <v>3</v>
+      </c>
       <c r="J30" s="46"/>
       <c r="K30" s="46"/>
       <c r="L30" s="46"/>
       <c r="M30" s="46"/>
       <c r="N30" s="46"/>
-      <c r="O30" s="46"/>
+      <c r="O30" s="18"/>
       <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="52"/>
       <c r="C31" s="25" t="s">
@@ -1994,19 +2327,24 @@
       <c r="F31" s="20">
         <v>30</v>
       </c>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
+      <c r="G31" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I31" s="52">
+        <v>3</v>
+      </c>
       <c r="J31" s="46"/>
       <c r="K31" s="46"/>
       <c r="L31" s="46"/>
       <c r="M31" s="46"/>
       <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
+      <c r="O31" s="18"/>
       <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="17"/>
       <c r="B32" s="20"/>
       <c r="C32" s="24" t="s">
@@ -2021,19 +2359,24 @@
       <c r="F32" s="20">
         <v>31</v>
       </c>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
+      <c r="G32" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I32" s="52">
+        <v>3</v>
+      </c>
       <c r="J32" s="46"/>
       <c r="K32" s="46"/>
       <c r="L32" s="46"/>
       <c r="M32" s="46"/>
       <c r="N32" s="46"/>
-      <c r="O32" s="46"/>
+      <c r="O32" s="18"/>
       <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="17"/>
       <c r="B33" s="20"/>
       <c r="C33" s="28" t="s">
@@ -2046,19 +2389,24 @@
       <c r="F33" s="20">
         <v>32</v>
       </c>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
+      <c r="G33" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I33" s="52">
+        <v>4</v>
+      </c>
       <c r="J33" s="46"/>
       <c r="K33" s="46"/>
       <c r="L33" s="46"/>
       <c r="M33" s="46"/>
       <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
+      <c r="O33" s="18"/>
       <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="17"/>
       <c r="B34" s="20"/>
       <c r="C34" s="6" t="s">
@@ -2071,19 +2419,24 @@
       <c r="F34" s="20">
         <v>33</v>
       </c>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
+      <c r="G34" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="H34" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I34" s="52">
+        <v>4</v>
+      </c>
       <c r="J34" s="46"/>
       <c r="K34" s="46"/>
       <c r="L34" s="46"/>
       <c r="M34" s="46"/>
       <c r="N34" s="46"/>
-      <c r="O34" s="46"/>
+      <c r="O34" s="18"/>
       <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="20"/>
       <c r="C35" s="6" t="s">
@@ -2098,19 +2451,24 @@
       <c r="F35" s="20">
         <v>34</v>
       </c>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
+      <c r="G35" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="H35" s="60" t="s">
+        <v>171</v>
+      </c>
+      <c r="I35" s="52">
+        <v>4</v>
+      </c>
       <c r="J35" s="46"/>
       <c r="K35" s="46"/>
       <c r="L35" s="46"/>
       <c r="M35" s="46"/>
       <c r="N35" s="46"/>
-      <c r="O35" s="46"/>
+      <c r="O35" s="18"/>
       <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="20"/>
       <c r="C36" s="6" t="s">
@@ -2123,19 +2481,24 @@
       <c r="F36" s="20">
         <v>35</v>
       </c>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
+      <c r="G36" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="H36" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I36" s="52">
+        <v>5</v>
+      </c>
       <c r="J36" s="46"/>
       <c r="K36" s="46"/>
       <c r="L36" s="46"/>
       <c r="M36" s="46"/>
       <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
+      <c r="O36" s="18"/>
       <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-    </row>
-    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="52"/>
       <c r="C37" s="6" t="s">
@@ -2150,19 +2513,24 @@
       <c r="F37" s="20">
         <v>36</v>
       </c>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
+      <c r="G37" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="H37" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="52">
+        <v>4</v>
+      </c>
       <c r="J37" s="46"/>
       <c r="K37" s="46"/>
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
       <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
+      <c r="O37" s="18"/>
       <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-    </row>
-    <row r="38" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="20"/>
       <c r="C38" s="6" t="s">
@@ -2177,19 +2545,24 @@
       <c r="F38" s="20">
         <v>37</v>
       </c>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="46"/>
+      <c r="G38" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I38" s="52">
+        <v>3</v>
+      </c>
       <c r="J38" s="46"/>
       <c r="K38" s="46"/>
       <c r="L38" s="46"/>
       <c r="M38" s="46"/>
       <c r="N38" s="46"/>
-      <c r="O38" s="46"/>
+      <c r="O38" s="18"/>
       <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="20"/>
       <c r="C39" s="27" t="s">
@@ -2202,19 +2575,24 @@
       <c r="F39" s="21">
         <v>38</v>
       </c>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
+      <c r="G39" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="H39" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I39" s="52">
+        <v>4</v>
+      </c>
       <c r="J39" s="46"/>
       <c r="K39" s="46"/>
       <c r="L39" s="46"/>
       <c r="M39" s="46"/>
       <c r="N39" s="46"/>
-      <c r="O39" s="46"/>
+      <c r="O39" s="18"/>
       <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-    </row>
-    <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="20"/>
       <c r="C40" s="6" t="s">
@@ -2229,19 +2607,24 @@
       <c r="F40" s="21">
         <v>39</v>
       </c>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
+      <c r="G40" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="H40" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I40" s="52">
+        <v>5</v>
+      </c>
       <c r="J40" s="46"/>
       <c r="K40" s="46"/>
       <c r="L40" s="46"/>
       <c r="M40" s="46"/>
       <c r="N40" s="46"/>
-      <c r="O40" s="46"/>
+      <c r="O40" s="18"/>
       <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="20"/>
       <c r="C41" s="6" t="s">
@@ -2256,19 +2639,24 @@
       <c r="F41" s="20">
         <v>40</v>
       </c>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
+      <c r="G41" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H41" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I41" s="52">
+        <v>4</v>
+      </c>
       <c r="J41" s="46"/>
       <c r="K41" s="46"/>
       <c r="L41" s="46"/>
       <c r="M41" s="46"/>
       <c r="N41" s="46"/>
-      <c r="O41" s="46"/>
+      <c r="O41" s="18"/>
       <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-    </row>
-    <row r="42" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
       <c r="B42" s="20"/>
       <c r="C42" s="29" t="s">
@@ -2281,19 +2669,24 @@
       <c r="F42" s="15">
         <v>41</v>
       </c>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
+      <c r="G42" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I42" s="52">
+        <v>3</v>
+      </c>
       <c r="J42" s="46"/>
       <c r="K42" s="46"/>
       <c r="L42" s="46"/>
       <c r="M42" s="46"/>
       <c r="N42" s="46"/>
-      <c r="O42" s="46"/>
+      <c r="O42" s="18"/>
       <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-    </row>
-    <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="20"/>
       <c r="C43" s="24" t="s">
@@ -2308,19 +2701,24 @@
       <c r="F43" s="15">
         <v>42</v>
       </c>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="46"/>
+      <c r="G43" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H43" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I43" s="52">
+        <v>3</v>
+      </c>
       <c r="J43" s="46"/>
       <c r="K43" s="46"/>
       <c r="L43" s="46"/>
       <c r="M43" s="46"/>
       <c r="N43" s="46"/>
-      <c r="O43" s="46"/>
+      <c r="O43" s="18"/>
       <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-    </row>
-    <row r="44" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="20"/>
       <c r="C44" s="25" t="s">
@@ -2335,19 +2733,24 @@
       <c r="F44" s="15">
         <v>43</v>
       </c>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
+      <c r="G44" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I44" s="52">
+        <v>4</v>
+      </c>
       <c r="J44" s="46"/>
       <c r="K44" s="46"/>
       <c r="L44" s="46"/>
       <c r="M44" s="46"/>
       <c r="N44" s="46"/>
-      <c r="O44" s="46"/>
+      <c r="O44" s="18"/>
       <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-    </row>
-    <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="20"/>
       <c r="C45" s="25" t="s">
@@ -2360,19 +2763,24 @@
       <c r="F45" s="15">
         <v>44</v>
       </c>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
+      <c r="G45" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I45" s="52">
+        <v>3</v>
+      </c>
       <c r="J45" s="46"/>
       <c r="K45" s="46"/>
       <c r="L45" s="46"/>
       <c r="M45" s="46"/>
       <c r="N45" s="46"/>
-      <c r="O45" s="46"/>
+      <c r="O45" s="18"/>
       <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-    </row>
-    <row r="46" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
       <c r="B46" s="52"/>
       <c r="C46" s="23" t="s">
@@ -2385,19 +2793,24 @@
       <c r="F46" s="15">
         <v>45</v>
       </c>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
+      <c r="G46" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H46" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="I46" s="52">
+        <v>3</v>
+      </c>
       <c r="J46" s="46"/>
       <c r="K46" s="46"/>
       <c r="L46" s="46"/>
       <c r="M46" s="46"/>
       <c r="N46" s="46"/>
-      <c r="O46" s="46"/>
+      <c r="O46" s="18"/>
       <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-    </row>
-    <row r="47" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="37"/>
       <c r="B47" s="20"/>
       <c r="C47" s="24" t="s">
@@ -2412,19 +2825,24 @@
       <c r="F47" s="15">
         <v>46</v>
       </c>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="46"/>
+      <c r="G47" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H47" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I47" s="52">
+        <v>3</v>
+      </c>
       <c r="J47" s="46"/>
       <c r="K47" s="46"/>
       <c r="L47" s="46"/>
       <c r="M47" s="46"/>
       <c r="N47" s="46"/>
-      <c r="O47" s="46"/>
+      <c r="O47" s="18"/>
       <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-    </row>
-    <row r="48" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="37"/>
       <c r="B48" s="52"/>
       <c r="C48" s="24" t="s">
@@ -2439,19 +2857,24 @@
       <c r="F48" s="15">
         <v>47</v>
       </c>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="46"/>
+      <c r="G48" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H48" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I48" s="52">
+        <v>4</v>
+      </c>
       <c r="J48" s="46"/>
       <c r="K48" s="46"/>
       <c r="L48" s="46"/>
       <c r="M48" s="46"/>
       <c r="N48" s="46"/>
-      <c r="O48" s="46"/>
+      <c r="O48" s="18"/>
       <c r="P48" s="18"/>
-      <c r="Q48" s="18"/>
-    </row>
-    <row r="49" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="37"/>
       <c r="B49" s="20"/>
       <c r="C49" s="25" t="s">
@@ -2464,19 +2887,24 @@
       <c r="F49" s="15">
         <v>48</v>
       </c>
-      <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="46"/>
+      <c r="G49" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H49" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I49" s="52">
+        <v>4</v>
+      </c>
       <c r="J49" s="46"/>
       <c r="K49" s="46"/>
       <c r="L49" s="46"/>
       <c r="M49" s="46"/>
       <c r="N49" s="46"/>
-      <c r="O49" s="46"/>
+      <c r="O49" s="18"/>
       <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-    </row>
-    <row r="50" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="37"/>
       <c r="B50" s="20"/>
       <c r="C50" s="25" t="s">
@@ -2491,19 +2919,24 @@
       <c r="F50" s="15">
         <v>49</v>
       </c>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="46"/>
+      <c r="G50" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="H50" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I50" s="52">
+        <v>3</v>
+      </c>
       <c r="J50" s="46"/>
       <c r="K50" s="46"/>
       <c r="L50" s="46"/>
       <c r="M50" s="46"/>
       <c r="N50" s="46"/>
-      <c r="O50" s="46"/>
+      <c r="O50" s="18"/>
       <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-    </row>
-    <row r="51" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="37"/>
       <c r="B51" s="52"/>
       <c r="C51" s="23" t="s">
@@ -2518,19 +2951,24 @@
       <c r="F51" s="15">
         <v>50</v>
       </c>
-      <c r="G51" s="46"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="46"/>
+      <c r="G51" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="H51" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="I51" s="52">
+        <v>3</v>
+      </c>
       <c r="J51" s="46"/>
       <c r="K51" s="46"/>
       <c r="L51" s="46"/>
       <c r="M51" s="46"/>
       <c r="N51" s="46"/>
-      <c r="O51" s="46"/>
+      <c r="O51" s="18"/>
       <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-    </row>
-    <row r="52" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="20"/>
       <c r="C52" s="27" t="s">
         <v>46</v>
@@ -2542,19 +2980,24 @@
       <c r="F52" s="15">
         <v>51</v>
       </c>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
+      <c r="G52" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="H52" s="60" t="s">
+        <v>158</v>
+      </c>
+      <c r="I52" s="52">
+        <v>3</v>
+      </c>
       <c r="J52" s="46"/>
       <c r="K52" s="46"/>
       <c r="L52" s="46"/>
       <c r="M52" s="46"/>
       <c r="N52" s="46"/>
-      <c r="O52" s="46"/>
+      <c r="O52" s="18"/>
       <c r="P52" s="18"/>
-      <c r="Q52" s="18"/>
-    </row>
-    <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="20"/>
       <c r="C53" s="25" t="s">
         <v>47</v>
@@ -2568,8 +3011,17 @@
       <c r="F53" s="15">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G53" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H53" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I53" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="20"/>
       <c r="C54" s="27" t="s">
         <v>48</v>
@@ -2581,8 +3033,17 @@
       <c r="F54" s="15">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G54" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H54" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I54" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="20"/>
       <c r="C55" s="25" t="s">
         <v>49</v>
@@ -2596,8 +3057,17 @@
       <c r="F55" s="15">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G55" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H55" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I55" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="20"/>
       <c r="C56" s="26" t="s">
         <v>50</v>
@@ -2609,8 +3079,17 @@
       <c r="F56" s="15">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G56" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H56" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I56" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="20"/>
       <c r="C57" s="23" t="s">
         <v>51</v>
@@ -2624,8 +3103,17 @@
       <c r="F57" s="15">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G57" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H57" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I57" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="22"/>
       <c r="C58" s="23" t="s">
         <v>52</v>
@@ -2639,8 +3127,17 @@
       <c r="F58" s="15">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G58" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H58" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I58" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="20"/>
       <c r="C59" s="25" t="s">
         <v>53</v>
@@ -2654,8 +3151,17 @@
       <c r="F59" s="15">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G59" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H59" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I59" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="20"/>
       <c r="C60" s="23" t="s">
         <v>54</v>
@@ -2667,8 +3173,17 @@
       <c r="F60" s="15">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G60" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I60" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="52"/>
       <c r="C61" s="26" t="s">
         <v>55</v>
@@ -2682,8 +3197,17 @@
       <c r="F61" s="22">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G61" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H61" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I61" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="52"/>
       <c r="C62" s="23" t="s">
         <v>56</v>
@@ -2697,8 +3221,17 @@
       <c r="F62" s="15">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G62" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H62" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I62" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="20"/>
       <c r="C63" s="24" t="s">
         <v>57</v>
@@ -2712,8 +3245,17 @@
       <c r="F63" s="15">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G63" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H63" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I63" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="20"/>
       <c r="C64" s="29" t="s">
         <v>58</v>
@@ -2725,8 +3267,17 @@
       <c r="F64" s="15">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G64" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H64" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I64" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="20"/>
       <c r="C65" s="24" t="s">
         <v>59</v>
@@ -2740,8 +3291,17 @@
       <c r="F65" s="15">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G65" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H65" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I65" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="52"/>
       <c r="C66" s="28" t="s">
         <v>60</v>
@@ -2755,8 +3315,17 @@
       <c r="F66" s="15">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G66" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="H66" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I66" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="20"/>
       <c r="C67" s="25" t="s">
         <v>61</v>
@@ -2770,8 +3339,17 @@
       <c r="F67" s="15">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G67" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H67" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I67" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="20"/>
       <c r="C68" s="27" t="s">
         <v>62</v>
@@ -2783,8 +3361,17 @@
       <c r="F68" s="15">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G68" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H68" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I68" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="20"/>
       <c r="C69" s="24" t="s">
         <v>63</v>
@@ -2798,8 +3385,17 @@
       <c r="F69" s="15">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G69" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H69" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I69" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="20"/>
       <c r="C70" s="23" t="s">
         <v>64</v>
@@ -2813,8 +3409,17 @@
       <c r="F70" s="15">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G70" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H70" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I70" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B71" s="20"/>
       <c r="C71" s="24" t="s">
         <v>65</v>
@@ -2828,8 +3433,17 @@
       <c r="F71" s="15">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G71" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H71" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I71" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="52"/>
       <c r="C72" s="33" t="s">
         <v>126</v>
@@ -2841,8 +3455,17 @@
       <c r="F72" s="15">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G72" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H72" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="I72" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="20"/>
       <c r="C73" s="32" t="s">
         <v>66</v>
@@ -2854,8 +3477,17 @@
       <c r="F73" s="15">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G73" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H73" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I73" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="20"/>
       <c r="C74" s="27" t="s">
         <v>67</v>
@@ -2869,8 +3501,17 @@
       <c r="F74" s="15">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G74" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H74" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I74" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="20"/>
       <c r="C75" s="24" t="s">
         <v>68</v>
@@ -2884,8 +3525,17 @@
       <c r="F75" s="15">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G75" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H75" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I75" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="20"/>
       <c r="C76" s="30" t="s">
         <v>69</v>
@@ -2897,8 +3547,17 @@
       <c r="F76" s="15">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G76" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H76" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I76" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="20"/>
       <c r="C77" s="24" t="s">
         <v>70</v>
@@ -2912,8 +3571,17 @@
       <c r="F77" s="15">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G77" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H77" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I77" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="20"/>
       <c r="C78" s="25" t="s">
         <v>71</v>
@@ -2927,8 +3595,17 @@
       <c r="F78" s="15">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G78" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H78" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I78" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="20"/>
       <c r="C79" s="25" t="s">
         <v>72</v>
@@ -2942,8 +3619,17 @@
       <c r="F79" s="15">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G79" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H79" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I79" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="20"/>
       <c r="C80" s="24" t="s">
         <v>73</v>
@@ -2955,8 +3641,17 @@
       <c r="F80" s="15">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G80" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H80" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I80" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="20"/>
       <c r="C81" s="24" t="s">
         <v>74</v>
@@ -2970,8 +3665,17 @@
       <c r="F81" s="15">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G81" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H81" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I81" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="20"/>
       <c r="C82" s="27" t="s">
         <v>118</v>
@@ -2985,8 +3689,17 @@
       <c r="F82" s="20">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G82" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H82" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I82" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="52"/>
       <c r="C83" s="25" t="s">
         <v>119</v>
@@ -3000,8 +3713,17 @@
       <c r="F83" s="20">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G83" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H83" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I83" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B84" s="20"/>
       <c r="C84" s="24" t="s">
         <v>120</v>
@@ -3013,8 +3735,17 @@
       <c r="F84" s="20">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G84" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H84" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I84" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B85" s="20"/>
       <c r="C85" s="25" t="s">
         <v>121</v>
@@ -3028,8 +3759,17 @@
       <c r="F85" s="20">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G85" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H85" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I85" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B86" s="52"/>
       <c r="C86" s="24" t="s">
         <v>122</v>
@@ -3043,8 +3783,17 @@
       <c r="F86" s="20">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G86" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H86" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I86" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B87" s="52"/>
       <c r="C87" s="24" t="s">
         <v>123</v>
@@ -3056,8 +3805,17 @@
       <c r="F87" s="20">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H87" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I87" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B88" s="52"/>
       <c r="C88" s="25" t="s">
         <v>124</v>
@@ -3071,8 +3829,17 @@
       <c r="F88" s="20">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G88" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H88" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I88" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B89" s="20"/>
       <c r="C89" s="27" t="s">
         <v>125</v>
@@ -3084,8 +3851,17 @@
       <c r="F89" s="20">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G89" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H89" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I89" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B90" s="20"/>
       <c r="C90" s="25" t="s">
         <v>79</v>
@@ -3097,8 +3873,17 @@
       <c r="F90" s="20">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G90" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H90" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I90" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B91" s="20"/>
       <c r="C91" s="24" t="s">
         <v>80</v>
@@ -3110,8 +3895,17 @@
       <c r="F91" s="20">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G91" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H91" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I91" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B92" s="20"/>
       <c r="C92" s="23" t="s">
         <v>81</v>
@@ -3125,8 +3919,17 @@
       <c r="F92" s="20">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G92" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H92" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I92" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B93" s="20"/>
       <c r="C93" s="27" t="s">
         <v>82</v>
@@ -3140,8 +3943,17 @@
       <c r="F93" s="20">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G93" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H93" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="I93" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B94" s="52"/>
       <c r="C94" s="25" t="s">
         <v>83</v>
@@ -3153,8 +3965,17 @@
       <c r="F94" s="20">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G94" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H94" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I94" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B95" s="52"/>
       <c r="C95" s="30" t="s">
         <v>84</v>
@@ -3166,8 +3987,17 @@
       <c r="F95" s="20">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G95" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H95" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I95" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B96" s="20"/>
       <c r="C96" s="25" t="s">
         <v>85</v>
@@ -3181,8 +4011,17 @@
       <c r="F96" s="20">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G96" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H96" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I96" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B97" s="52"/>
       <c r="C97" s="29" t="s">
         <v>86</v>
@@ -3194,8 +4033,17 @@
       <c r="F97" s="20">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G97" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H97" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I97" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B98" s="20"/>
       <c r="C98" s="25" t="s">
         <v>87</v>
@@ -3207,8 +4055,17 @@
       <c r="F98" s="20">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G98" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H98" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I98" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B99" s="20"/>
       <c r="C99" s="30" t="s">
         <v>88</v>
@@ -3222,8 +4079,17 @@
       <c r="F99" s="20">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G99" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H99" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I99" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B100" s="20"/>
       <c r="C100" s="30" t="s">
         <v>89</v>
@@ -3237,8 +4103,17 @@
       <c r="F100" s="20">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G100" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H100" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I100" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B101" s="20"/>
       <c r="C101" s="25" t="s">
         <v>90</v>
@@ -3252,8 +4127,17 @@
       <c r="F101" s="20">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G101" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H101" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I101" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B102" s="20"/>
       <c r="C102" s="23" t="s">
         <v>91</v>
@@ -3267,8 +4151,17 @@
       <c r="F102" s="20">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G102" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H102" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I102" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B103" s="52"/>
       <c r="C103" s="26" t="s">
         <v>92</v>
@@ -3280,8 +4173,17 @@
       <c r="F103" s="20">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G103" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H103" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I103" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B104" s="20"/>
       <c r="C104" s="24" t="s">
         <v>93</v>
@@ -3293,8 +4195,17 @@
       <c r="F104" s="20">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G104" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H104" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I104" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B105" s="20"/>
       <c r="C105" s="24" t="s">
         <v>94</v>
@@ -3308,8 +4219,17 @@
       <c r="F105" s="20">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G105" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H105" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="I105" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B106" s="20"/>
       <c r="C106" s="25" t="s">
         <v>95</v>
@@ -3321,8 +4241,17 @@
       <c r="F106" s="20">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G106" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H106" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I106" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="20"/>
       <c r="C107" s="25" t="s">
         <v>96</v>
@@ -3334,8 +4263,17 @@
       <c r="F107" s="20">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G107" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H107" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I107" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B108" s="20"/>
       <c r="C108" s="30" t="s">
         <v>97</v>
@@ -3349,8 +4287,17 @@
       <c r="F108" s="20">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G108" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="H108" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I108" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B109" s="52"/>
       <c r="C109" s="30" t="s">
         <v>98</v>
@@ -3362,8 +4309,17 @@
       <c r="F109" s="21">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G109" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H109" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I109" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B110" s="20"/>
       <c r="C110" s="30" t="s">
         <v>99</v>
@@ -3375,8 +4331,17 @@
       <c r="F110" s="20">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G110" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H110" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I110" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B111" s="20"/>
       <c r="C111" s="31" t="s">
         <v>100</v>
@@ -3388,8 +4353,17 @@
       <c r="F111" s="20">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G111" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H111" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="I111" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B112" s="52"/>
       <c r="C112" s="24" t="s">
         <v>101</v>
@@ -3403,8 +4377,17 @@
       <c r="F112" s="20">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G112" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H112" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="I112" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B113" s="20"/>
       <c r="C113" s="24" t="s">
         <v>111</v>
@@ -3418,8 +4401,17 @@
       <c r="F113" s="20">
         <v>121</v>
       </c>
-    </row>
-    <row r="114" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G113" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H113" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I113" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B114" s="52"/>
       <c r="C114" s="24" t="s">
         <v>103</v>
@@ -3433,8 +4425,17 @@
       <c r="F114" s="20">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G114" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H114" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I114" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B115" s="20"/>
       <c r="C115" s="25" t="s">
         <v>104</v>
@@ -3448,8 +4449,17 @@
       <c r="F115" s="20">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G115" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H115" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I115" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B116" s="20"/>
       <c r="C116" s="30" t="s">
         <v>105</v>
@@ -3463,8 +4473,17 @@
       <c r="F116" s="20">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G116" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H116" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I116" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="20"/>
       <c r="C117" s="27" t="s">
         <v>106</v>
@@ -3478,8 +4497,17 @@
       <c r="F117" s="20">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G117" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H117" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I117" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B118" s="20"/>
       <c r="C118" s="29" t="s">
         <v>107</v>
@@ -3493,8 +4521,17 @@
       <c r="F118" s="20">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G118" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H118" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I118" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B119" s="20"/>
       <c r="C119" s="29" t="s">
         <v>108</v>
@@ -3508,8 +4545,17 @@
       <c r="F119" s="20">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G119" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H119" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I119" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B120" s="20"/>
       <c r="C120" s="34" t="s">
         <v>109</v>
@@ -3521,8 +4567,17 @@
       <c r="F120" s="20">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G120" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H120" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I120" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B121" s="52"/>
       <c r="C121" s="30" t="s">
         <v>110</v>
@@ -3534,8 +4589,17 @@
       <c r="F121" s="20">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G121" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H121" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I121" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B122" s="52"/>
       <c r="C122" s="29" t="s">
         <v>0</v>
@@ -3549,8 +4613,17 @@
       <c r="F122" s="20">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G122" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H122" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="I122" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B123" s="20"/>
       <c r="C123" s="24" t="s">
         <v>112</v>
@@ -3564,8 +4637,17 @@
       <c r="F123" s="20">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G123" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="H123" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I123" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B124" s="20"/>
       <c r="C124" s="24" t="s">
         <v>113</v>
@@ -3577,8 +4659,17 @@
       <c r="F124" s="20">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G124" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H124" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I124" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B125" s="52"/>
       <c r="C125" s="27" t="s">
         <v>114</v>
@@ -3590,8 +4681,17 @@
       <c r="F125" s="20">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G125" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H125" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="I125" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B126" s="20"/>
       <c r="C126" s="26" t="s">
         <v>115</v>
@@ -3603,8 +4703,17 @@
       <c r="F126" s="21">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G126" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H126" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I126" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B127" s="20"/>
       <c r="C127" s="27" t="s">
         <v>116</v>
@@ -3616,8 +4725,17 @@
       <c r="F127" s="20">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G127" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H127" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I127" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B128" s="20"/>
       <c r="C128" s="23" t="s">
         <v>117</v>
@@ -3631,8 +4749,17 @@
       <c r="F128" s="20">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G128" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H128" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I128" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B129" s="20"/>
       <c r="C129" s="24" t="s">
         <v>132</v>
@@ -3644,8 +4771,17 @@
       <c r="F129" s="20">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G129" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H129" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I129" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B130" s="52"/>
       <c r="C130" s="27" t="s">
         <v>133</v>
@@ -3659,8 +4795,17 @@
       <c r="F130" s="20">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G130" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H130" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="I130" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B131" s="20"/>
       <c r="C131" s="24" t="s">
         <v>134</v>
@@ -3672,8 +4817,17 @@
       <c r="F131" s="20">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G131" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H131" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="I131" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B132" s="52"/>
       <c r="C132" s="27" t="s">
         <v>135</v>
@@ -3685,8 +4839,17 @@
       <c r="F132" s="20">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G132" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H132" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I132" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B133" s="20"/>
       <c r="C133" s="24" t="s">
         <v>136</v>
@@ -3700,8 +4863,17 @@
       <c r="F133" s="20">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G133" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H133" s="59" t="s">
+        <v>162</v>
+      </c>
+      <c r="I133" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B134" s="52"/>
       <c r="C134" s="41" t="s">
         <v>137</v>
@@ -3713,8 +4885,17 @@
       <c r="F134" s="20">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G134" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H134" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I134" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B135" s="20"/>
       <c r="C135" s="41" t="s">
         <v>138</v>
@@ -3726,8 +4907,17 @@
       <c r="F135" s="20">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G135" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H135" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="I135" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B136" s="20"/>
       <c r="C136" s="42" t="s">
         <v>139</v>
@@ -3739,8 +4929,17 @@
       <c r="F136" s="20">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G136" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H136" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I136" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B137" s="20"/>
       <c r="C137" s="44" t="s">
         <v>140</v>
@@ -3754,8 +4953,17 @@
       <c r="F137" s="20">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G137" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H137" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I137" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B138" s="20"/>
       <c r="C138" s="44" t="s">
         <v>141</v>
@@ -3769,8 +4977,23 @@
       <c r="F138" s="20">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G138" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="H138" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I138" s="15">
+        <v>3</v>
+      </c>
+      <c r="J138" s="50" t="s">
+        <v>201</v>
+      </c>
+      <c r="K138" s="50" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="139" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B139" s="52"/>
       <c r="C139" s="41" t="s">
         <v>142</v>
@@ -3784,8 +5007,23 @@
       <c r="F139" s="20">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G139" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H139" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I139" s="15">
+        <v>4</v>
+      </c>
+      <c r="J139" s="50" t="s">
+        <v>199</v>
+      </c>
+      <c r="K139" s="50" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="140" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B140" s="20"/>
       <c r="C140" s="44" t="s">
         <v>143</v>
@@ -3799,8 +5037,23 @@
       <c r="F140" s="20">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G140" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H140" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I140" s="15">
+        <v>2</v>
+      </c>
+      <c r="J140" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="K140" s="50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="141" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B141" s="20"/>
       <c r="C141" s="43" t="s">
         <v>144</v>
@@ -3814,8 +5067,23 @@
       <c r="F141" s="15">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G141" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H141" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I141" s="15">
+        <v>3</v>
+      </c>
+      <c r="J141" s="61" t="s">
+        <v>197</v>
+      </c>
+      <c r="K141" s="61" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="142" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C142" s="38" t="s">
         <v>145</v>
       </c>
@@ -3825,12 +5093,26 @@
       <c r="E142" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F142" s="53">
+      <c r="F142" s="20">
         <v>141</v>
       </c>
-      <c r="G142" s="53"/>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G142" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H142" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I142" s="15">
+        <v>4</v>
+      </c>
+      <c r="J142" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="K142" s="50" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="143" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C143" s="38" t="s">
         <v>146</v>
       </c>
@@ -3840,12 +5122,26 @@
       <c r="E143" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F143" s="53">
+      <c r="F143" s="20">
         <v>142</v>
       </c>
-      <c r="G143" s="53"/>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G143" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H143" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="I143" s="15">
+        <v>3</v>
+      </c>
+      <c r="J143" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="K143" s="50" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="144" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C144" s="38" t="s">
         <v>147</v>
       </c>
@@ -3855,12 +5151,26 @@
       <c r="E144" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F144" s="53">
+      <c r="F144" s="20">
         <v>143</v>
       </c>
-      <c r="G144" s="53"/>
-    </row>
-    <row r="145" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G144" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="H144" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I144" s="15">
+        <v>3</v>
+      </c>
+      <c r="J144" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="K144" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="145" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C145" s="38" t="s">
         <v>148</v>
       </c>
@@ -3870,13 +5180,27 @@
       <c r="E145" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F145" s="53">
+      <c r="F145" s="20">
         <v>144</v>
       </c>
-      <c r="G145" s="53"/>
-    </row>
-    <row r="146" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C146" s="54" t="s">
+      <c r="G145" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="H145" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="I145" s="15">
+        <v>3</v>
+      </c>
+      <c r="J145" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="K145" s="50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="146" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C146" s="53" t="s">
         <v>149</v>
       </c>
       <c r="D146" s="38" t="s">
@@ -3885,12 +5209,26 @@
       <c r="E146" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F146" s="53">
+      <c r="F146" s="20">
         <v>145</v>
       </c>
-      <c r="G146" s="53"/>
-    </row>
-    <row r="147" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G146" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H146" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I146" s="15">
+        <v>4</v>
+      </c>
+      <c r="J146" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="K146" s="50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="147" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C147" s="38" t="s">
         <v>150</v>
       </c>
@@ -3900,23 +5238,46 @@
       <c r="E147" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="F147" s="53">
+      <c r="F147" s="20">
         <v>146</v>
       </c>
-      <c r="G147" s="53"/>
-    </row>
-    <row r="148" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C148" s="55" t="s">
+      <c r="G147" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H147" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I147" s="15">
+        <v>3</v>
+      </c>
+      <c r="J147" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="K147" s="50" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="148" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C148" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D148" s="13" t="s">
+      <c r="D148" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="E148" s="13" t="s">
+      <c r="E148" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="F148" s="13">
+      <c r="F148" s="15">
         <v>147</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H148" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="I148" s="15" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>